<commit_message>
second version of erd
</commit_message>
<xml_diff>
--- a/PropERD.xlsx
+++ b/PropERD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\ProP_Sems2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B077A4-F23A-4FC5-9646-864C23C48DEF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFD43FA-F82E-4658-9F4B-7BB6343F86F2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{F9329643-C742-4494-8F74-C9DF6F4FE0C1}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
   <si>
     <t>User</t>
   </si>
@@ -199,17 +198,41 @@
     <t>cSpotNr (pk)</t>
   </si>
   <si>
-    <t>Loan entity</t>
-  </si>
-  <si>
     <t>TransactionType</t>
+  </si>
+  <si>
+    <t>(deposit/ food/ items/ loan/ registration/ camp)</t>
+  </si>
+  <si>
+    <t>articleNr (pk)</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>Condition (working / broken)</t>
+  </si>
+  <si>
+    <t>TransactionID (pk)</t>
+  </si>
+  <si>
+    <t>articleNr (pk) (fk)</t>
+  </si>
+  <si>
+    <t>articleType</t>
+  </si>
+  <si>
+    <t>TransactionID (pk) (fk)</t>
+  </si>
+  <si>
+    <t>Loan entity (intersection)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,8 +268,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,6 +309,11 @@
         <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -304,22 +339,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="Accent1" xfId="5" builtinId="29"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Input" xfId="4" builtinId="20"/>
@@ -795,10 +833,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{762E0458-5D2F-4C28-B240-45A732488928}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I14:I15"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,7 +847,7 @@
     <col min="4" max="4" width="28.140625" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" customWidth="1"/>
     <col min="6" max="6" width="22.5703125" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" customWidth="1"/>
+    <col min="7" max="7" width="33.42578125" customWidth="1"/>
     <col min="8" max="8" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -905,7 +943,7 @@
         <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -919,7 +957,7 @@
         <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -930,7 +968,7 @@
         <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -938,25 +976,28 @@
         <v>31</v>
       </c>
       <c r="F14" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F16" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B17" t="s">
+      <c r="F17" s="5" t="s">
         <v>55</v>
+      </c>
+      <c r="G17" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -969,7 +1010,20 @@
         <v>53</v>
       </c>
     </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F20" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>63</v>
+      </c>
       <c r="H22">
         <v>1</v>
       </c>
@@ -978,6 +1032,26 @@
       </c>
       <c r="J22">
         <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F25" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>